<commit_message>
Added beginning of doc describing ISL budget
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM2.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM2.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>Units</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Downlink Frequency</t>
   </si>
   <si>
-    <t>UHF Downlink</t>
-  </si>
-  <si>
     <t>Spacecraft Losses</t>
   </si>
   <si>
@@ -187,6 +184,24 @@
   </si>
   <si>
     <t>Dumbo TX power</t>
+  </si>
+  <si>
+    <t>monopole</t>
+  </si>
+  <si>
+    <t>downlink</t>
+  </si>
+  <si>
+    <t>uplink</t>
+  </si>
+  <si>
+    <t>dipole</t>
+  </si>
+  <si>
+    <t>turnstile</t>
+  </si>
+  <si>
+    <t>VHF Downlink</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,9 +1035,10 @@
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1035,7 +1051,7 @@
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1050,9 +1066,9 @@
       </c>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>6</v>
@@ -1064,7 +1080,7 @@
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1093,7 @@
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
     </row>
-    <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -1092,7 +1108,7 @@
       </c>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1122,7 @@
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
@@ -1114,12 +1130,12 @@
         <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
@@ -1133,7 +1149,7 @@
       <c r="D8" s="13"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
@@ -1145,8 +1161,11 @@
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
@@ -1159,8 +1178,17 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10">
+        <v>4.7</v>
+      </c>
+      <c r="H10">
+        <v>72.489999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
@@ -1169,12 +1197,21 @@
       </c>
       <c r="C11" s="21">
         <f>C6-SUM(C7:C8,C10)</f>
-        <v>-89.722341194960094</v>
+        <v>-89.822341194960089</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11">
+        <v>6.8</v>
+      </c>
+      <c r="H11">
+        <v>63.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1187,8 +1224,11 @@
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1197,12 +1237,21 @@
       </c>
       <c r="C13" s="21">
         <f>C11-C7-k+C12</f>
-        <v>117.51125373165709</v>
+        <v>117.3112537316571</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+      <c r="H13">
+        <v>81.290000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -1215,8 +1264,17 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>64.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
@@ -1225,12 +1283,15 @@
       </c>
       <c r="C15" s="24">
         <f>C13-C14</f>
-        <v>81.490653818377467</v>
+        <v>81.290653818377479</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1241,8 +1302,17 @@
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16">
+        <v>0.3</v>
+      </c>
+      <c r="H16">
+        <v>81.290000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>26</v>
       </c>
@@ -1250,17 +1320,25 @@
         <v>4</v>
       </c>
       <c r="C17" s="6">
-        <f>udf</f>
-        <v>440</v>
+        <v>145</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>64.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>6</v>
@@ -1272,7 +1350,7 @@
       <c r="D18" s="13"/>
       <c r="E18" s="30"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>7</v>
       </c>
@@ -1286,9 +1364,9 @@
       <c r="D19" s="13"/>
       <c r="E19" s="30"/>
     </row>
-    <row r="20" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>6</v>
@@ -1302,7 +1380,7 @@
       </c>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
@@ -1316,7 +1394,7 @@
       <c r="D21" s="13"/>
       <c r="E21" s="11"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>13</v>
       </c>
@@ -1324,12 +1402,12 @@
         <v>6</v>
       </c>
       <c r="C22" s="21">
-        <v>0.2</v>
+        <v>6.8</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>14</v>
       </c>
@@ -1337,13 +1415,12 @@
         <v>6</v>
       </c>
       <c r="C23" s="31">
-        <f>loss</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>15</v>
       </c>
@@ -1356,7 +1433,7 @@
       <c r="D24" s="13"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>17</v>
       </c>
@@ -1365,26 +1442,26 @@
       </c>
       <c r="C25" s="21">
         <f>22+20*LOG10((C24*1000)/(c_/(C17*10^6)))</f>
-        <v>99.312041238320276</v>
+        <v>89.670347753296028</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="21">
         <f>C21-SUM(C22:C23,C25)</f>
-        <v>-89.722341194960094</v>
+        <v>-86.580647709935846</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>19</v>
       </c>
@@ -1398,7 +1475,7 @@
       <c r="D27" s="13"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -1407,12 +1484,12 @@
       </c>
       <c r="C28" s="21">
         <f>C26-C22-k+C27</f>
-        <v>117.51125373165709</v>
+        <v>114.05294721668133</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1503,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="9" t="s">
         <v>24</v>
       </c>
@@ -1435,12 +1512,12 @@
       </c>
       <c r="C30" s="24">
         <f>C28-C29</f>
-        <v>67.511253731657092</v>
+        <v>64.052947216681332</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Just adding a few more tidbits of info
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM2.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM2.xlsx
@@ -418,9 +418,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -490,6 +487,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal 1" xfId="1"/>
@@ -729,8 +729,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,138 +1046,138 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>440</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <f>10*LOG(5)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>5</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="16">
         <v>2</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <f>C3+C4-C5</f>
         <v>9.9897000433601875</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="11"/>
+      <c r="C7" s="5">
+        <v>4.7</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f>loss</f>
         <v>0.2</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>5</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
       <c r="G9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <f>22+20*LOG10((C9*1000)/(c_/(C2*10^6)))</f>
         <v>99.312041238320276</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="10"/>
       <c r="F10" t="s">
         <v>33</v>
       </c>
@@ -1189,18 +1189,18 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <f>C6-SUM(C7:C8,C10)</f>
-        <v>-89.822341194960089</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="11"/>
+        <v>-94.222341194960094</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="10"/>
       <c r="F11" t="s">
         <v>32</v>
       </c>
@@ -1212,35 +1212,35 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <f>C4-C5-10*LOG(SSNT)</f>
         <v>-21.166405073382808</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="10"/>
       <c r="G12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <f>C11-C7-k+C12</f>
-        <v>117.3112537316571</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="11"/>
+        <v>108.51125373165709</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="10"/>
       <c r="F13" t="s">
         <v>33</v>
       </c>
@@ -1252,18 +1252,18 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <f>10*LOG(ul)</f>
         <v>36.020599913279625</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="10"/>
       <c r="F14" t="s">
         <v>32</v>
       </c>
@@ -1275,18 +1275,18 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <f>C13-C14</f>
-        <v>81.290653818377479</v>
-      </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="11"/>
+        <v>72.490653818377467</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="10"/>
       <c r="G15" t="s">
         <v>35</v>
       </c>
@@ -1295,13 +1295,13 @@
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="26">
+      <c r="B16" s="5"/>
+      <c r="C16" s="25">
         <f>0.5*ERFC(2*(C15/SQRT(2)))</f>
         <v>0</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
       <c r="F16" t="s">
         <v>33</v>
       </c>
@@ -1313,19 +1313,19 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>145</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="7"/>
       <c r="F17" t="s">
         <v>32</v>
       </c>
@@ -1337,197 +1337,197 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="28">
         <f>10*LOG(5)</f>
         <v>6.9897000433601884</v>
       </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="30"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <f>SCG</f>
         <v>5</v>
       </c>
-      <c r="D19" s="13"/>
-      <c r="E19" s="30"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <f>SCL</f>
         <v>2</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <f>C18+C19-C20</f>
         <v>9.9897000433601875</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>6.8</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="30">
         <v>0.1</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="18">
         <v>5</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <f>22+20*LOG10((C24*1000)/(c_/(C17*10^6)))</f>
         <v>89.670347753296028</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <f>C21-SUM(C22:C23,C25)</f>
         <v>-86.580647709935846</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="20">
         <f>C19-C20-10*LOG(SSNT)</f>
         <v>-21.166405073382808</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="20">
         <f>C26-C22-k+C27</f>
         <v>114.05294721668133</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="21">
         <f>10*LOG(udl)</f>
         <v>50</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="23">
         <f>C28-C29</f>
         <v>64.052947216681332</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="26">
+      <c r="B31" s="5"/>
+      <c r="C31" s="25">
         <f>0.5*ERFC(2*(C30/SQRT(2)))</f>
         <v>0</v>
       </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="28"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixed a conversion fuck up
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM2.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM2.xlsx
@@ -1,19 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9720" windowHeight="7320"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="AIL">#REF!</definedName>
     <definedName name="alt">#REF!</definedName>
@@ -676,12 +673,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1058,7 +1049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1164,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>0.30000000000000004</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="12"/>
@@ -1176,9 +1169,8 @@
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="e">
-        <f>loss</f>
-        <v>#REF!</v>
+      <c r="C8" s="6">
+        <v>0.2</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="12"/>
@@ -1229,9 +1221,9 @@
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="22" t="e">
+      <c r="C11" s="22">
         <f>C6-SUM(C7:C8,C10)</f>
-        <v>#REF!</v>
+        <v>-87.170347753296028</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="12"/>
@@ -1252,9 +1244,9 @@
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="22" t="e">
-        <f>C4-C5-10*LOG(SSNT)</f>
-        <v>#REF!</v>
+      <c r="C12" s="22">
+        <f>C4-C5-10*LOG(261)</f>
+        <v>-21.166405073382808</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="12"/>
@@ -1269,9 +1261,9 @@
       <c r="B13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="22" t="e">
+      <c r="C13" s="22">
         <f>C11-C7--228.6+C12</f>
-        <v>#REF!</v>
+        <v>119.96324717332118</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12"/>
@@ -1315,9 +1307,9 @@
       <c r="B15" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="25" t="e">
+      <c r="C15" s="25">
         <f>C13-C14</f>
-        <v>#REF!</v>
+        <v>83.942647260041554</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="12"/>
@@ -1330,9 +1322,9 @@
         <v>31</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="27" t="e">
+      <c r="C16" s="27">
         <f>0.5*ERFC(2*(C15/SQRT(2)))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
@@ -1391,9 +1383,8 @@
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="e">
-        <f>SCG</f>
-        <v>#REF!</v>
+      <c r="C19" s="6">
+        <v>5</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="30"/>
@@ -1405,9 +1396,8 @@
       <c r="B20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="18" t="e">
-        <f>SCL</f>
-        <v>#REF!</v>
+      <c r="C20" s="18">
+        <v>2</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>11</v>
@@ -1421,9 +1411,9 @@
       <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="22" t="e">
+      <c r="C21" s="22">
         <f>C18+C19-C20</f>
-        <v>#REF!</v>
+        <v>3</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="12"/>
@@ -1436,7 +1426,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="22">
-        <v>0.1</v>
+        <v>6.8</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="12"/>
@@ -1449,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="31">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
@@ -1488,9 +1478,9 @@
       <c r="B26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="22" t="e">
+      <c r="C26" s="22">
         <f>C21-SUM(C22:C23,C25)</f>
-        <v>#REF!</v>
+        <v>-103.21204123832028</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="12"/>
@@ -1502,9 +1492,9 @@
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="22" t="e">
-        <f>C19-C20-10*LOG(SSNT)</f>
-        <v>#REF!</v>
+      <c r="C27" s="22">
+        <f>C19-C20-10*LOG(261)</f>
+        <v>-21.166405073382808</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="12"/>
@@ -1516,9 +1506,9 @@
       <c r="B28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="22" t="e">
+      <c r="C28" s="22">
         <f>C26-C22--228.6+C27</f>
-        <v>#REF!</v>
+        <v>97.42155368829691</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="12"/>
@@ -1544,9 +1534,9 @@
       <c r="B30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="25" t="e">
+      <c r="C30" s="25">
         <f>C28-C29</f>
-        <v>#REF!</v>
+        <v>61.400953775017285</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="12"/>
@@ -1556,9 +1546,9 @@
         <v>31</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="27" t="e">
+      <c r="C31" s="27">
         <f>0.5*ERFC(2*(C30/SQRT(2)))</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
       <c r="D31" s="32"/>
       <c r="E31" s="29"/>

</xml_diff>

<commit_message>
Fixed a brain fart
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM2.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6">
-        <v>145</v>
+        <v>440</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>5</v>
@@ -1101,8 +1101,8 @@
         <v>7</v>
       </c>
       <c r="C3" s="10">
-        <f>10*LOG(1)</f>
-        <v>0</v>
+        <f>10*LOG(5)</f>
+        <v>6.9897000433601884</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="C6" s="10">
         <f>C3+C4-C5</f>
-        <v>3</v>
+        <v>9.9897000433601875</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
@@ -1157,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="6">
-        <v>0.3</v>
+        <v>4.7</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="12"/>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="C10" s="22">
         <f>22+20*LOG10((C9*1000)/(299792400/(C2*10^6)))</f>
-        <v>89.670347753296028</v>
+        <v>99.312041238320276</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="12"/>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="C11" s="22">
         <f>C6-SUM(C7:C8,C10)</f>
-        <v>-87.170347753296028</v>
+        <v>-94.222341194960094</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="12"/>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="C13" s="22">
         <f>C11-C7--228.6+C12</f>
-        <v>119.96324717332118</v>
+        <v>108.51125373165709</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="12"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="C15" s="25">
         <f>C13-C14</f>
-        <v>83.942647260041554</v>
+        <v>72.490653818377467</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="12"/>
@@ -1346,7 +1346,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="6">
-        <v>440</v>
+        <v>145</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>33</v>
@@ -1439,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="31">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C25" s="22">
         <f>22+20*LOG10((C24*1000)/(299792400/(C17*10^6)))</f>
-        <v>99.312041238320276</v>
+        <v>89.670347753296028</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="C26" s="22">
         <f>C21-SUM(C22:C23,C25)</f>
-        <v>-103.21204123832028</v>
+        <v>-93.670347753296028</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="12"/>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C28" s="22">
         <f>C26-C22--228.6+C27</f>
-        <v>97.42155368829691</v>
+        <v>106.96324717332118</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="12"/>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="C30" s="25">
         <f>C28-C29</f>
-        <v>61.400953775017285</v>
+        <v>70.942647260041554</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="12"/>

</xml_diff>